<commit_message>
add heritage events and containers to indvidual report, #757
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/individual_report_template.xlsx
+++ b/bio_diversity/static/report_templates/individual_report_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Event History" sheetId="1" r:id="rId1"/>
@@ -433,14 +433,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
@@ -496,8 +496,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -544,13 +548,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -588,6 +593,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
expand individual report, #814
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/individual_report_template.xlsx
+++ b/bio_diversity/static/report_templates/individual_report_template.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Event History" sheetId="1" r:id="rId1"/>
     <sheet name="Heritage" sheetId="2" r:id="rId2"/>
     <sheet name="Containers" sheetId="3" r:id="rId3"/>
     <sheet name="Treatments" sheetId="4" r:id="rId4"/>
+    <sheet name="Details" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Individual Report:</t>
   </si>
@@ -87,6 +88,33 @@
   </si>
   <si>
     <t>Treatement</t>
+  </si>
+  <si>
+    <t>Containers</t>
+  </si>
+  <si>
+    <t>Individual:</t>
+  </si>
+  <si>
+    <t>Dose</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Individual Treatments:</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Subjective Value</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -145,11 +173,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -549,7 +579,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,24 +615,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection sqref="A1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -611,6 +651,75 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean up redundent code in reports and maps view
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/individual_report_template.xlsx
+++ b/bio_diversity/static/report_templates/individual_report_template.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Event History" sheetId="1" r:id="rId1"/>
     <sheet name="Heritage" sheetId="2" r:id="rId2"/>
     <sheet name="Containers" sheetId="3" r:id="rId3"/>
-    <sheet name="Treatments" sheetId="4" r:id="rId4"/>
-    <sheet name="Details" sheetId="5" r:id="rId5"/>
+    <sheet name="Details" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Individual Report:</t>
   </si>
@@ -84,16 +83,7 @@
     <t>Direction</t>
   </si>
   <si>
-    <t>Treatments</t>
-  </si>
-  <si>
     <t>Treatement</t>
-  </si>
-  <si>
-    <t>Containers</t>
-  </si>
-  <si>
-    <t>Individual:</t>
   </si>
   <si>
     <t>Dose</t>
@@ -615,65 +605,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,12 +620,12 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -698,13 +633,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>6</v>
@@ -713,13 +648,13 @@
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="K4" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add comments to reports
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/individual_report_template.xlsx
+++ b/bio_diversity/static/report_templates/individual_report_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Event History" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Individual Report:</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Duration (mins)</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -583,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,30 +650,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -686,16 +690,19 @@
       <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="F4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>